<commit_message>
added docker to architecture picture
</commit_message>
<xml_diff>
--- a/Architecture.xlsx
+++ b/Architecture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Master PC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernh\Documents\GitHub\cc-task3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9954750E-EEBC-4DC5-9827-0306064B7C70}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1344E982-30ED-4AE4-87D5-46599730C484}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5DA0DBE-3305-4B0C-BE79-37A10F1A6995}"/>
+    <workbookView xWindow="28680" yWindow="-2055" windowWidth="29040" windowHeight="15840" xr2:uid="{D5DA0DBE-3305-4B0C-BE79-37A10F1A6995}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1157,15 +1157,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:colOff>171450</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1180,7 +1180,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4019550" y="1390650"/>
+          <a:off x="3981450" y="1381125"/>
           <a:ext cx="4752975" cy="4438650"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -1211,6 +1211,609 @@
           <a:r>
             <a:rPr lang="de-DE" sz="1100"/>
             <a:t>Docker</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rechteck: abgerundete Ecken 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBE25D4A-5185-466B-AD25-0AE0B818B55F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5648325" y="2038350"/>
+          <a:ext cx="1485900" cy="828675"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-AT" sz="1100"/>
+            <a:t>Koordinator</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Rechteck: abgerundete Ecken 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DD72847-BBAB-48F6-9528-C4A8E79C34E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5667375" y="3124200"/>
+          <a:ext cx="1485900" cy="828675"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-AT" sz="1100"/>
+            <a:t>RabbitMQ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Gerade Verbindung mit Pfeil 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CC2FB17-3D7E-4E33-A9E6-C9D44C2B12D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="24" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6400800" y="2886075"/>
+          <a:ext cx="9525" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Gerade Verbindung mit Pfeil 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8AC22B6-0954-4AE5-A081-F9A76FE5A81C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="24" idx="2"/>
+          <a:endCxn id="31" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6391275" y="3952875"/>
+          <a:ext cx="19050" cy="447675"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="Rechteck: abgerundete Ecken 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{169002D2-724A-44D3-B5B3-5551101EF357}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5934075" y="4400550"/>
+          <a:ext cx="1314450" cy="742950"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-AT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="Rechteck 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9553830A-EE02-4B9C-85DD-97DEF7417E6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6257925" y="1828800"/>
+          <a:ext cx="219075" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="Rechteck 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75B29DC6-93CE-4EC8-8C78-69AB7422232C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6886574" y="1523999"/>
+          <a:ext cx="1143001" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1050"/>
+            <a:t>HTTP 55551/upload</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>414338</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Gerade Verbindung mit Pfeil 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15E70C31-6F98-4DCB-B57D-06841A3A1A50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="16" idx="0"/>
+          <a:endCxn id="38" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="3712369" y="912020"/>
+          <a:ext cx="1533525" cy="3557587"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="Rechteck: abgerundete Ecken 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83194F4E-04AB-47A5-B4A1-49ECBF9A0E03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5857875" y="4400550"/>
+          <a:ext cx="1314450" cy="742950"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-AT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Rechteck: abgerundete Ecken 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54FBF7F3-B4C2-4E37-BF51-8069E65E6B47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5734050" y="4400550"/>
+          <a:ext cx="1314450" cy="742950"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-AT" sz="1100"/>
+            <a:t>Worker</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>

</xml_diff>

<commit_message>
added wroker and koordinator to architecture description
</commit_message>
<xml_diff>
--- a/Architecture.xlsx
+++ b/Architecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernh\Documents\GitHub\cc-task3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1344E982-30ED-4AE4-87D5-46599730C484}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0CADDC-89A5-4361-A3AA-1723EBD8357A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2055" windowWidth="29040" windowHeight="15840" xr2:uid="{D5DA0DBE-3305-4B0C-BE79-37A10F1A6995}"/>
   </bookViews>
@@ -2123,7 +2123,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+      <selection activeCell="A2" sqref="A2:U41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>